<commit_message>
ultimas modificaciones del codigo de pp y figuras
</commit_message>
<xml_diff>
--- a/plot/tabla_climatologiapp_epoca_sis.xlsx
+++ b/plot/tabla_climatologiapp_epoca_sis.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>SIS CÁLIDO</t>
-  </si>
-  <si>
-    <t>SIS FRÍO</t>
-  </si>
-  <si>
-    <t>media</t>
+    <t>SIS-ESTIVAL</t>
+  </si>
+  <si>
+    <t>SIS-INVERNAL</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
   <si>
     <t>Std</t>
@@ -40,7 +40,7 @@
     <t>P99</t>
   </si>
   <si>
-    <t>Max</t>
+    <t>Máx</t>
   </si>
 </sst>
 </file>

</xml_diff>